<commit_message>
plot residual slopes by session
</commit_message>
<xml_diff>
--- a/data/habituationStats.xlsx
+++ b/data/habituationStats.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianahaggerty/Documents/MATLAB/projects/blinkCNSAnalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA48D74-B521-B34A-B137-CF5A189DC9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C9FF0C-A12C-5F45-BB38-23C8BCAC5322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34340" yWindow="7780" windowWidth="10000" windowHeight="17440" xr2:uid="{28A2D6F7-8163-E449-8D12-69ABA47417E5}"/>
+    <workbookView xWindow="34340" yWindow="7780" windowWidth="10000" windowHeight="17440" activeTab="1" xr2:uid="{28A2D6F7-8163-E449-8D12-69ABA47417E5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="byTrial" sheetId="1" r:id="rId1"/>
+    <sheet name="byAcquisition" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>t-stat</t>
   </si>
@@ -438,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16520FA2-BA3D-D549-822D-F967E632F85E}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,4 +622,193 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518A30D2-D533-5841-BFB1-CC93424FEE2A}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>0.4773</v>
+      </c>
+      <c r="C2">
+        <v>-9.4999999999999998E-3</v>
+      </c>
+      <c r="D2">
+        <v>-2.5297999999999998</v>
+      </c>
+      <c r="E2">
+        <v>2.4E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>-2.3199999999999998E-2</v>
+      </c>
+      <c r="C3">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="D3">
+        <v>1.097</v>
+      </c>
+      <c r="E3">
+        <v>0.29120000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>-0.13039999999999999</v>
+      </c>
+      <c r="C4">
+        <v>-2.52E-2</v>
+      </c>
+      <c r="D4">
+        <v>-4.4953000000000003</v>
+      </c>
+      <c r="E4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>-5.6800000000000003E-2</v>
+      </c>
+      <c r="C5">
+        <v>-7.7200000000000005E-2</v>
+      </c>
+      <c r="D5">
+        <v>-4.3287000000000004</v>
+      </c>
+      <c r="E5">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0.47</v>
+      </c>
+      <c r="C6">
+        <v>0.2374</v>
+      </c>
+      <c r="D6">
+        <v>0.20430000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.84099999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.27889999999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.1166</v>
+      </c>
+      <c r="D7">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.84899999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.4304</v>
+      </c>
+      <c r="C8">
+        <v>-0.31619999999999998</v>
+      </c>
+      <c r="D8">
+        <v>-2.3397999999999999</v>
+      </c>
+      <c r="E8">
+        <v>3.4599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>5.8299999999999998E-2</v>
+      </c>
+      <c r="C9">
+        <v>7.6755000000000004</v>
+      </c>
+      <c r="D9">
+        <v>1.6463000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.12189999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.79869999999999997</v>
+      </c>
+      <c r="C10">
+        <v>-2.6700000000000002E-2</v>
+      </c>
+      <c r="D10">
+        <v>-2.3955000000000002</v>
+      </c>
+      <c r="E10">
+        <v>3.1099999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>